<commit_message>
lab 3.03 with questions
</commit_message>
<xml_diff>
--- a/physics/lab303/к лабе.xlsx
+++ b/physics/lab303/к лабе.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\docs_for_labs\physics\lab303\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE94063A-6F0A-439D-B236-D6F8838F5E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90BDE6A-ECF3-456A-A795-C824ABE71A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -191,9 +191,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -206,18 +206,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -362,7 +360,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -373,11 +371,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -609,7 +607,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -620,11 +618,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent5"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -844,6 +842,134 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-722A-4C31-991B-79486714567A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>I_кр1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист2!$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>220.43299999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист2!$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.26319999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8CA8-44DA-ADA3-81625BE83A8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>I_кр2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист2!$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>227.14100000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист2!$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.31574649999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8CA8-44DA-ADA3-81625BE83A8D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1132,10 +1258,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.57306671041119861"/>
-          <c:y val="0.1672448235637212"/>
-          <c:w val="0.3547110673665792"/>
-          <c:h val="0.22627369495479732"/>
+          <c:x val="0.66910156399206056"/>
+          <c:y val="0.16724492872858041"/>
+          <c:w val="0.23240123571330099"/>
+          <c:h val="0.34130110027564059"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2077,10 +2203,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.8129600002499995</c:v>
+                  <c:v>6.4786401000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.2203175836200986</c:v>
+                  <c:v>6.8790435999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2333,13 +2459,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -4004,16 +4127,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>251011</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>531718</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>17369</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4040,16 +4163,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>33336</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>31376</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>10925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>350744</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139512</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4116,7 +4239,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4124,34 +4247,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -4376,10 +4499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB21D727-DED0-4439-9626-39350150CB64}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4436,19 +4559,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="I2" s="8">
-        <f>A3-A2</f>
+        <f t="shared" ref="I2:I32" si="0">A3-A2</f>
         <v>20</v>
       </c>
       <c r="J2">
-        <f>ABS(B2-B3)</f>
+        <f t="shared" ref="J2:J32" si="1">ABS(B2-B3)</f>
         <v>3.0000000000002247E-4</v>
       </c>
       <c r="L2" s="8">
-        <f>A3-A2</f>
+        <f t="shared" ref="L2:L32" si="2">A3-A2</f>
         <v>20</v>
       </c>
       <c r="M2" s="1">
-        <f>ABS(C3-C2)</f>
+        <f t="shared" ref="M2:M32" si="3">ABS(C3-C2)</f>
         <v>2.0000000000003348E-4</v>
       </c>
       <c r="O2" t="s">
@@ -4470,27 +4593,34 @@
         <v>0.34360000000000002</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D33" si="0">B3/A3</f>
+        <f t="shared" ref="D3:D33" si="4">B3/A3</f>
         <v>1.3989999999999999E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E33" si="1">C3/A3</f>
+        <f t="shared" ref="E3:E33" si="5">C3/A3</f>
         <v>1.7180000000000001E-2</v>
       </c>
+      <c r="F3">
+        <f>F4*1000</f>
+        <v>220433</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.26319999999999999</v>
+      </c>
       <c r="I3" s="8">
-        <f>A4-A3</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="J3">
-        <f>ABS(B3-B4)</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="L3" s="8">
-        <f>A4-A3</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M3" s="1">
-        <f>ABS(C4-C3)</f>
+        <f t="shared" si="3"/>
         <v>1.9999999999997797E-4</v>
       </c>
       <c r="O3" t="s">
@@ -4504,7 +4634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>40</v>
       </c>
@@ -4515,27 +4645,30 @@
         <v>0.34379999999999999</v>
       </c>
       <c r="D4">
+        <f t="shared" si="4"/>
+        <v>6.9974999999999994E-3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="5"/>
+        <v>8.5950000000000002E-3</v>
+      </c>
+      <c r="F4" s="13">
+        <v>220.43299999999999</v>
+      </c>
+      <c r="I4" s="8">
         <f t="shared" si="0"/>
-        <v>6.9974999999999994E-3</v>
-      </c>
-      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="1"/>
-        <v>8.5950000000000002E-3</v>
-      </c>
-      <c r="I4" s="8">
-        <f>A5-A4</f>
-        <v>20</v>
-      </c>
-      <c r="J4">
-        <f>ABS(B4-B5)</f>
         <v>1.000000000000445E-4</v>
       </c>
       <c r="L4" s="8">
-        <f>A5-A4</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M4" s="1">
-        <f>ABS(C5-C4)</f>
+        <f t="shared" si="3"/>
         <v>5.9999999999998943E-4</v>
       </c>
     </row>
@@ -4550,27 +4683,27 @@
         <v>0.34320000000000001</v>
       </c>
       <c r="D5">
+        <f t="shared" si="4"/>
+        <v>4.6666666666666671E-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="5"/>
+        <v>5.7200000000000003E-3</v>
+      </c>
+      <c r="I5" s="8">
         <f t="shared" si="0"/>
-        <v>4.6666666666666671E-3</v>
-      </c>
-      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="1"/>
-        <v>5.7200000000000003E-3</v>
-      </c>
-      <c r="I5" s="8">
-        <f>A6-A5</f>
-        <v>20</v>
-      </c>
-      <c r="J5">
-        <f>ABS(B5-B6)</f>
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="L5" s="8">
-        <f>A6-A5</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M5" s="1">
-        <f>ABS(C6-C5)</f>
+        <f t="shared" si="3"/>
         <v>3.0000000000002247E-4</v>
       </c>
     </row>
@@ -4585,31 +4718,31 @@
         <v>0.34350000000000003</v>
       </c>
       <c r="D6">
+        <f t="shared" si="4"/>
+        <v>3.5062500000000003E-3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="5"/>
+        <v>4.2937500000000007E-3</v>
+      </c>
+      <c r="I6" s="8">
         <f t="shared" si="0"/>
-        <v>3.5062500000000003E-3</v>
-      </c>
-      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="1"/>
-        <v>4.2937500000000007E-3</v>
-      </c>
-      <c r="I6" s="8">
-        <f>A7-A6</f>
-        <v>20</v>
-      </c>
-      <c r="J6">
-        <f>ABS(B6-B7)</f>
         <v>3.9999999999995595E-4</v>
       </c>
       <c r="L6" s="8">
-        <f>A7-A6</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M6" s="1">
-        <f>ABS(C7-C6)</f>
+        <f t="shared" si="3"/>
         <v>1.9999999999997797E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>100</v>
       </c>
@@ -4620,27 +4753,30 @@
         <v>0.34370000000000001</v>
       </c>
       <c r="D7">
+        <f t="shared" si="4"/>
+        <v>2.8089999999999999E-3</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="5"/>
+        <v>3.437E-3</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.22714100000000001</v>
+      </c>
+      <c r="I7" s="8">
         <f t="shared" si="0"/>
-        <v>2.8089999999999999E-3</v>
-      </c>
-      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="1"/>
-        <v>3.437E-3</v>
-      </c>
-      <c r="I7" s="8">
-        <f>A8-A7</f>
-        <v>20</v>
-      </c>
-      <c r="J7">
-        <f>ABS(B7-B8)</f>
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="L7" s="8">
-        <f>A8-A7</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M7" s="1">
-        <f>ABS(C8-C7)</f>
+        <f t="shared" si="3"/>
         <v>7.999999999999674E-4</v>
       </c>
     </row>
@@ -4655,27 +4791,35 @@
         <v>0.34449999999999997</v>
       </c>
       <c r="D8">
+        <f t="shared" si="4"/>
+        <v>2.3449999999999999E-3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="5"/>
+        <v>2.8708333333333333E-3</v>
+      </c>
+      <c r="F8">
+        <f>F7*1000</f>
+        <v>227.14100000000002</v>
+      </c>
+      <c r="G8" s="1">
+        <f>AVERAGE(C13:C14)*1.03</f>
+        <v>0.31574649999999999</v>
+      </c>
+      <c r="I8" s="8">
         <f t="shared" si="0"/>
-        <v>2.3449999999999999E-3</v>
-      </c>
-      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="1"/>
-        <v>2.8708333333333333E-3</v>
-      </c>
-      <c r="I8" s="8">
-        <f>A9-A8</f>
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <f>ABS(B8-B9)</f>
         <v>4.0000000000001146E-4</v>
       </c>
       <c r="L8" s="8">
-        <f>A9-A8</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M8" s="1">
-        <f>ABS(C9-C8)</f>
+        <f t="shared" si="3"/>
         <v>1.1000000000000454E-3</v>
       </c>
     </row>
@@ -4690,27 +4834,27 @@
         <v>0.34560000000000002</v>
       </c>
       <c r="D9">
+        <f t="shared" si="4"/>
+        <v>2.0128571428571426E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="5"/>
+        <v>2.4685714285714289E-3</v>
+      </c>
+      <c r="I9" s="8">
         <f t="shared" si="0"/>
-        <v>2.0128571428571426E-3</v>
-      </c>
-      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="1"/>
-        <v>2.4685714285714289E-3</v>
-      </c>
-      <c r="I9" s="8">
-        <f>A10-A9</f>
-        <v>20</v>
-      </c>
-      <c r="J9">
-        <f>ABS(B9-B10)</f>
         <v>3.0000000000002247E-4</v>
       </c>
       <c r="L9" s="8">
-        <f>A10-A9</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M9" s="1">
-        <f>ABS(C10-C9)</f>
+        <f t="shared" si="3"/>
         <v>1.9999999999997797E-4</v>
       </c>
     </row>
@@ -4725,27 +4869,27 @@
         <v>0.3458</v>
       </c>
       <c r="D10">
+        <f t="shared" si="4"/>
+        <v>1.7593749999999999E-3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="5"/>
+        <v>2.16125E-3</v>
+      </c>
+      <c r="I10" s="8">
         <f t="shared" si="0"/>
-        <v>1.7593749999999999E-3</v>
-      </c>
-      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="1"/>
-        <v>2.16125E-3</v>
-      </c>
-      <c r="I10" s="8">
-        <f>A11-A10</f>
-        <v>20</v>
-      </c>
-      <c r="J10">
-        <f>ABS(B10-B11)</f>
         <v>1.4999999999999458E-3</v>
       </c>
       <c r="L10" s="8">
-        <f>A11-A10</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M10" s="1">
-        <f>ABS(C11-C10)</f>
+        <f t="shared" si="3"/>
         <v>1.4000000000000123E-3</v>
       </c>
     </row>
@@ -4760,27 +4904,27 @@
         <v>0.34439999999999998</v>
       </c>
       <c r="D11">
+        <f t="shared" si="4"/>
+        <v>1.5555555555555557E-3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="5"/>
+        <v>1.9133333333333333E-3</v>
+      </c>
+      <c r="I11" s="8">
         <f t="shared" si="0"/>
-        <v>1.5555555555555557E-3</v>
-      </c>
-      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="1"/>
-        <v>1.9133333333333333E-3</v>
-      </c>
-      <c r="I11" s="8">
-        <f>A12-A11</f>
-        <v>20</v>
-      </c>
-      <c r="J11">
-        <f>ABS(B11-B12)</f>
         <v>3.9000000000000146E-3</v>
       </c>
       <c r="L11" s="8">
-        <f>A12-A11</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M11" s="1">
-        <f>ABS(C12-C11)</f>
+        <f t="shared" si="3"/>
         <v>6.2999999999999723E-3</v>
       </c>
     </row>
@@ -4795,27 +4939,27 @@
         <v>0.33810000000000001</v>
       </c>
       <c r="D12">
+        <f t="shared" si="4"/>
+        <v>1.3805E-3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="5"/>
+        <v>1.6905000000000002E-3</v>
+      </c>
+      <c r="I12" s="8">
         <f t="shared" si="0"/>
-        <v>1.3805E-3</v>
-      </c>
-      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="1"/>
-        <v>1.6905000000000002E-3</v>
-      </c>
-      <c r="I12" s="8">
-        <f>A13-A12</f>
-        <v>20</v>
-      </c>
-      <c r="J12">
-        <f>ABS(B12-B13)</f>
         <v>1.2900000000000023E-2</v>
       </c>
       <c r="L12" s="8">
-        <f>A13-A12</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M12" s="1">
-        <f>ABS(C13-C12)</f>
+        <f t="shared" si="3"/>
         <v>1.7699999999999994E-2</v>
       </c>
     </row>
@@ -4830,27 +4974,27 @@
         <v>0.32040000000000002</v>
       </c>
       <c r="D13">
+        <f t="shared" si="4"/>
+        <v>1.1963636363636362E-3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="5"/>
+        <v>1.4563636363636365E-3</v>
+      </c>
+      <c r="I13" s="8">
         <f t="shared" si="0"/>
-        <v>1.1963636363636362E-3</v>
-      </c>
-      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="1"/>
-        <v>1.4563636363636365E-3</v>
-      </c>
-      <c r="I13" s="12">
-        <f>A14-A13</f>
-        <v>20</v>
-      </c>
-      <c r="J13" s="13">
-        <f>ABS(B13-B14)</f>
         <v>4.1399999999999992E-2</v>
       </c>
       <c r="L13" s="8">
-        <f>A14-A13</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M13" s="1">
-        <f>ABS(C14-C13)</f>
+        <f t="shared" si="3"/>
         <v>2.7700000000000002E-2</v>
       </c>
     </row>
@@ -4865,34 +5009,34 @@
         <v>0.29270000000000002</v>
       </c>
       <c r="D14">
+        <f t="shared" si="4"/>
+        <v>9.2416666666666667E-4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="5"/>
+        <v>1.2195833333333334E-3</v>
+      </c>
+      <c r="I14" s="9">
         <f t="shared" si="0"/>
-        <v>9.2416666666666667E-4</v>
-      </c>
-      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="J14" s="10">
         <f t="shared" si="1"/>
-        <v>1.2195833333333334E-3</v>
-      </c>
-      <c r="I14" s="9">
-        <f>A15-A14</f>
-        <v>20</v>
-      </c>
-      <c r="J14" s="10">
-        <f>ABS(B14-B15)</f>
         <v>6.0099999999999987E-2</v>
       </c>
       <c r="L14" s="9">
-        <f>A15-A14</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M14" s="11">
-        <f>ABS(C15-C14)</f>
+        <f t="shared" si="3"/>
         <v>8.0100000000000005E-2</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14" t="s">
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4907,36 +5051,36 @@
         <v>0.21260000000000001</v>
       </c>
       <c r="D15">
+        <f t="shared" si="4"/>
+        <v>6.2192307692307699E-4</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="5"/>
+        <v>8.1769230769230769E-4</v>
+      </c>
+      <c r="I15" s="9">
         <f t="shared" si="0"/>
-        <v>6.2192307692307699E-4</v>
-      </c>
-      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="J15" s="10">
         <f t="shared" si="1"/>
-        <v>8.1769230769230769E-4</v>
-      </c>
-      <c r="I15" s="9">
-        <f>A16-A15</f>
-        <v>20</v>
-      </c>
-      <c r="J15" s="10">
-        <f>ABS(B15-B16)</f>
         <v>2.2199999999999998E-2</v>
       </c>
       <c r="L15" s="9">
-        <f>A16-A15</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M15" s="11">
-        <f>ABS(C16-C15)</f>
+        <f t="shared" si="3"/>
         <v>3.0100000000000016E-2</v>
       </c>
-      <c r="O15" s="14">
-        <v>20</v>
-      </c>
-      <c r="P15" s="14" t="s">
+      <c r="O15" s="12">
+        <v>20</v>
+      </c>
+      <c r="P15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="Q15" s="12">
         <f>-J14</f>
         <v>-6.0099999999999987E-2</v>
       </c>
@@ -4952,27 +5096,27 @@
         <v>0.1825</v>
       </c>
       <c r="D16">
+        <f t="shared" si="4"/>
+        <v>4.9821428571428575E-4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="5"/>
+        <v>6.5178571428571423E-4</v>
+      </c>
+      <c r="I16" s="8">
         <f t="shared" si="0"/>
-        <v>4.9821428571428575E-4</v>
-      </c>
-      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="1"/>
-        <v>6.5178571428571423E-4</v>
-      </c>
-      <c r="I16" s="8">
-        <f>A17-A16</f>
-        <v>20</v>
-      </c>
-      <c r="J16">
-        <f>ABS(B16-B17)</f>
         <v>1.9500000000000017E-2</v>
       </c>
       <c r="L16" s="8">
-        <f>A17-A16</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M16" s="1">
-        <f>ABS(C17-C16)</f>
+        <f t="shared" si="3"/>
         <v>2.5700000000000001E-2</v>
       </c>
     </row>
@@ -4987,27 +5131,27 @@
         <v>0.15679999999999999</v>
       </c>
       <c r="D17">
+        <f t="shared" si="4"/>
+        <v>3.9999999999999996E-4</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="5"/>
+        <v>5.2266666666666661E-4</v>
+      </c>
+      <c r="I17" s="8">
         <f t="shared" si="0"/>
-        <v>3.9999999999999996E-4</v>
-      </c>
-      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="1"/>
-        <v>5.2266666666666661E-4</v>
-      </c>
-      <c r="I17" s="8">
-        <f>A18-A17</f>
-        <v>20</v>
-      </c>
-      <c r="J17">
-        <f>ABS(B17-B18)</f>
         <v>1.0399999999999993E-2</v>
       </c>
       <c r="L17" s="8">
-        <f>A18-A17</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M17" s="1">
-        <f>ABS(C18-C17)</f>
+        <f t="shared" si="3"/>
         <v>1.2300000000000005E-2</v>
       </c>
     </row>
@@ -5022,34 +5166,34 @@
         <v>0.14449999999999999</v>
       </c>
       <c r="D18">
+        <f t="shared" si="4"/>
+        <v>3.4250000000000003E-4</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="5"/>
+        <v>4.5156249999999998E-4</v>
+      </c>
+      <c r="I18" s="8">
         <f t="shared" si="0"/>
-        <v>3.4250000000000003E-4</v>
-      </c>
-      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="1"/>
-        <v>4.5156249999999998E-4</v>
-      </c>
-      <c r="I18" s="8">
-        <f>A19-A18</f>
-        <v>20</v>
-      </c>
-      <c r="J18">
-        <f>ABS(B18-B19)</f>
         <v>1.2300000000000005E-2</v>
       </c>
       <c r="L18" s="8">
-        <f>A19-A18</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M18" s="1">
-        <f>ABS(C19-C18)</f>
+        <f t="shared" si="3"/>
         <v>1.0499999999999982E-2</v>
       </c>
-      <c r="O18" s="14" t="s">
+      <c r="O18" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14" t="s">
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5064,36 +5208,36 @@
         <v>0.13400000000000001</v>
       </c>
       <c r="D19">
+        <f t="shared" si="4"/>
+        <v>2.8617647058823528E-4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="5"/>
+        <v>3.9411764705882355E-4</v>
+      </c>
+      <c r="I19" s="8">
         <f t="shared" si="0"/>
-        <v>2.8617647058823528E-4</v>
-      </c>
-      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="1"/>
-        <v>3.9411764705882355E-4</v>
-      </c>
-      <c r="I19" s="8">
-        <f>A20-A19</f>
-        <v>20</v>
-      </c>
-      <c r="J19">
-        <f>ABS(B19-B20)</f>
         <v>9.999999999999995E-3</v>
       </c>
       <c r="L19" s="8">
-        <f>A20-A19</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M19" s="1">
-        <f>ABS(C20-C19)</f>
+        <f t="shared" si="3"/>
         <v>1.3300000000000006E-2</v>
       </c>
-      <c r="O19" s="14">
-        <v>20</v>
-      </c>
-      <c r="P19" s="14" t="s">
+      <c r="O19" s="12">
+        <v>20</v>
+      </c>
+      <c r="P19" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q19" s="12">
         <v>8.0100000000000005E-2</v>
       </c>
     </row>
@@ -5108,27 +5252,27 @@
         <v>0.1207</v>
       </c>
       <c r="D20">
+        <f t="shared" si="4"/>
+        <v>2.4250000000000001E-4</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="5"/>
+        <v>3.3527777777777777E-4</v>
+      </c>
+      <c r="I20" s="8">
         <f t="shared" si="0"/>
-        <v>2.4250000000000001E-4</v>
-      </c>
-      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="1"/>
-        <v>3.3527777777777777E-4</v>
-      </c>
-      <c r="I20" s="8">
-        <f>A21-A20</f>
-        <v>20</v>
-      </c>
-      <c r="J20">
-        <f>ABS(B20-B21)</f>
         <v>1.0599999999999998E-2</v>
       </c>
       <c r="L20" s="8">
-        <f>A21-A20</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M20" s="1">
-        <f>ABS(C21-C20)</f>
+        <f t="shared" si="3"/>
         <v>1.6E-2</v>
       </c>
     </row>
@@ -5143,27 +5287,27 @@
         <v>0.1047</v>
       </c>
       <c r="D21">
+        <f t="shared" si="4"/>
+        <v>2.018421052631579E-4</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="5"/>
+        <v>2.7552631578947368E-4</v>
+      </c>
+      <c r="I21" s="8">
         <f t="shared" si="0"/>
-        <v>2.018421052631579E-4</v>
-      </c>
-      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="1"/>
-        <v>2.7552631578947368E-4</v>
-      </c>
-      <c r="I21" s="8">
-        <f>A22-A21</f>
-        <v>20</v>
-      </c>
-      <c r="J21">
-        <f>ABS(B21-B22)</f>
         <v>7.8000000000000014E-3</v>
       </c>
       <c r="L21" s="8">
-        <f>A22-A21</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M21" s="1">
-        <f>ABS(C22-C21)</f>
+        <f t="shared" si="3"/>
         <v>7.0999999999999952E-3</v>
       </c>
     </row>
@@ -5178,27 +5322,27 @@
         <v>9.7600000000000006E-2</v>
       </c>
       <c r="D22">
+        <f t="shared" si="4"/>
+        <v>1.7225000000000001E-4</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="5"/>
+        <v>2.4400000000000002E-4</v>
+      </c>
+      <c r="I22" s="8">
         <f t="shared" si="0"/>
-        <v>1.7225000000000001E-4</v>
-      </c>
-      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="1"/>
-        <v>2.4400000000000002E-4</v>
-      </c>
-      <c r="I22" s="8">
-        <f>A23-A22</f>
-        <v>20</v>
-      </c>
-      <c r="J22">
-        <f>ABS(B22-B23)</f>
         <v>6.3E-3</v>
       </c>
       <c r="L22" s="8">
-        <f>A23-A22</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M22" s="1">
-        <f>ABS(C23-C22)</f>
+        <f t="shared" si="3"/>
         <v>1.1300000000000004E-2</v>
       </c>
     </row>
@@ -5213,27 +5357,27 @@
         <v>8.6300000000000002E-2</v>
       </c>
       <c r="D23">
+        <f t="shared" si="4"/>
+        <v>1.4904761904761904E-4</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="5"/>
+        <v>2.0547619047619049E-4</v>
+      </c>
+      <c r="I23" s="8">
         <f t="shared" si="0"/>
-        <v>1.4904761904761904E-4</v>
-      </c>
-      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="1"/>
-        <v>2.0547619047619049E-4</v>
-      </c>
-      <c r="I23" s="8">
-        <f>A24-A23</f>
-        <v>20</v>
-      </c>
-      <c r="J23">
-        <f>ABS(B23-B24)</f>
         <v>4.8000000000000057E-3</v>
       </c>
       <c r="L23" s="8">
-        <f>A24-A23</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M23" s="1">
-        <f>ABS(C24-C23)</f>
+        <f t="shared" si="3"/>
         <v>6.3E-3</v>
       </c>
     </row>
@@ -5248,27 +5392,27 @@
         <v>0.08</v>
       </c>
       <c r="D24">
+        <f t="shared" si="4"/>
+        <v>1.3136363636363636E-4</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="5"/>
+        <v>1.8181818181818183E-4</v>
+      </c>
+      <c r="I24" s="8">
         <f t="shared" si="0"/>
-        <v>1.3136363636363636E-4</v>
-      </c>
-      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="1"/>
-        <v>1.8181818181818183E-4</v>
-      </c>
-      <c r="I24" s="8">
-        <f>A25-A24</f>
-        <v>20</v>
-      </c>
-      <c r="J24">
-        <f>ABS(B24-B25)</f>
         <v>5.5999999999999939E-3</v>
       </c>
       <c r="L24" s="8">
-        <f>A25-A24</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M24" s="1">
-        <f>ABS(C25-C24)</f>
+        <f t="shared" si="3"/>
         <v>5.9000000000000025E-3</v>
       </c>
     </row>
@@ -5283,27 +5427,27 @@
         <v>7.4099999999999999E-2</v>
       </c>
       <c r="D25">
+        <f t="shared" si="4"/>
+        <v>1.1347826086956522E-4</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="5"/>
+        <v>1.6108695652173913E-4</v>
+      </c>
+      <c r="I25" s="8">
         <f t="shared" si="0"/>
-        <v>1.1347826086956522E-4</v>
-      </c>
-      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="1"/>
-        <v>1.6108695652173913E-4</v>
-      </c>
-      <c r="I25" s="8">
-        <f>A26-A25</f>
-        <v>20</v>
-      </c>
-      <c r="J25">
-        <f>ABS(B25-B26)</f>
         <v>3.4000000000000002E-3</v>
       </c>
       <c r="L25" s="8">
-        <f>A26-A25</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M25" s="1">
-        <f>ABS(C26-C25)</f>
+        <f t="shared" si="3"/>
         <v>6.3E-3</v>
       </c>
     </row>
@@ -5318,27 +5462,27 @@
         <v>6.7799999999999999E-2</v>
       </c>
       <c r="D26">
+        <f t="shared" si="4"/>
+        <v>1.0166666666666667E-4</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="5"/>
+        <v>1.4124999999999999E-4</v>
+      </c>
+      <c r="I26" s="8">
         <f t="shared" si="0"/>
-        <v>1.0166666666666667E-4</v>
-      </c>
-      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="1"/>
-        <v>1.4124999999999999E-4</v>
-      </c>
-      <c r="I26" s="8">
-        <f>A27-A26</f>
-        <v>20</v>
-      </c>
-      <c r="J26">
-        <f>ABS(B26-B27)</f>
         <v>3.3000000000000043E-3</v>
       </c>
       <c r="L26" s="8">
-        <f>A27-A26</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M26" s="1">
-        <f>ABS(C27-C26)</f>
+        <f t="shared" si="3"/>
         <v>4.9000000000000016E-3</v>
       </c>
     </row>
@@ -5353,27 +5497,27 @@
         <v>6.2899999999999998E-2</v>
       </c>
       <c r="D27">
+        <f t="shared" si="4"/>
+        <v>9.1000000000000003E-5</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="5"/>
+        <v>1.2579999999999999E-4</v>
+      </c>
+      <c r="I27" s="8">
         <f t="shared" si="0"/>
-        <v>9.1000000000000003E-5</v>
-      </c>
-      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="1"/>
-        <v>1.2579999999999999E-4</v>
-      </c>
-      <c r="I27" s="8">
-        <f>A28-A27</f>
-        <v>20</v>
-      </c>
-      <c r="J27">
-        <f>ABS(B27-B28)</f>
         <v>2.5000000000000022E-3</v>
       </c>
       <c r="L27" s="8">
-        <f>A28-A27</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M27" s="1">
-        <f>ABS(C28-C27)</f>
+        <f t="shared" si="3"/>
         <v>4.8999999999999946E-3</v>
       </c>
     </row>
@@ -5388,27 +5532,27 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D28">
+        <f t="shared" si="4"/>
+        <v>8.2692307692307682E-5</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="5"/>
+        <v>1.1153846153846154E-4</v>
+      </c>
+      <c r="I28" s="8">
         <f t="shared" si="0"/>
-        <v>8.2692307692307682E-5</v>
-      </c>
-      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="J28">
         <f t="shared" si="1"/>
-        <v>1.1153846153846154E-4</v>
-      </c>
-      <c r="I28" s="8">
-        <f>A29-A28</f>
-        <v>20</v>
-      </c>
-      <c r="J28">
-        <f>ABS(B28-B29)</f>
         <v>2.5999999999999981E-3</v>
       </c>
       <c r="L28" s="8">
-        <f>A29-A28</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M28" s="1">
-        <f>ABS(C29-C28)</f>
+        <f t="shared" si="3"/>
         <v>3.2000000000000015E-3</v>
       </c>
     </row>
@@ -5423,27 +5567,27 @@
         <v>5.4800000000000001E-2</v>
       </c>
       <c r="D29">
+        <f t="shared" si="4"/>
+        <v>7.4814814814814815E-5</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="5"/>
+        <v>1.0148148148148149E-4</v>
+      </c>
+      <c r="I29" s="8">
         <f t="shared" si="0"/>
-        <v>7.4814814814814815E-5</v>
-      </c>
-      <c r="E29">
+        <v>20</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="1"/>
-        <v>1.0148148148148149E-4</v>
-      </c>
-      <c r="I29" s="8">
-        <f>A30-A29</f>
-        <v>20</v>
-      </c>
-      <c r="J29">
-        <f>ABS(B29-B30)</f>
         <v>2.3999999999999994E-3</v>
       </c>
       <c r="L29" s="8">
-        <f>A30-A29</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M29" s="1">
-        <f>ABS(C30-C29)</f>
+        <f t="shared" si="3"/>
         <v>3.0999999999999986E-3</v>
       </c>
     </row>
@@ -5458,27 +5602,27 @@
         <v>5.1700000000000003E-2</v>
       </c>
       <c r="D30">
+        <f t="shared" si="4"/>
+        <v>6.7857142857142861E-5</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="5"/>
+        <v>9.2321428571428575E-5</v>
+      </c>
+      <c r="I30" s="8">
         <f t="shared" si="0"/>
-        <v>6.7857142857142861E-5</v>
-      </c>
-      <c r="E30">
+        <v>20</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="1"/>
-        <v>9.2321428571428575E-5</v>
-      </c>
-      <c r="I30" s="8">
-        <f>A31-A30</f>
-        <v>20</v>
-      </c>
-      <c r="J30">
-        <f>ABS(B30-B31)</f>
         <v>1.799999999999996E-3</v>
       </c>
       <c r="L30" s="8">
-        <f>A31-A30</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M30" s="1">
-        <f>ABS(C31-C30)</f>
+        <f t="shared" si="3"/>
         <v>2.4000000000000063E-3</v>
       </c>
     </row>
@@ -5493,30 +5637,30 @@
         <v>4.9299999999999997E-2</v>
       </c>
       <c r="D31">
+        <f t="shared" si="4"/>
+        <v>6.2413793103448286E-5</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="5"/>
+        <v>8.4999999999999993E-5</v>
+      </c>
+      <c r="I31" s="8">
         <f t="shared" si="0"/>
-        <v>6.2413793103448286E-5</v>
-      </c>
-      <c r="E31">
+        <v>20</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="1"/>
-        <v>8.4999999999999993E-5</v>
-      </c>
-      <c r="I31" s="8">
-        <f>A32-A31</f>
-        <v>20</v>
-      </c>
-      <c r="J31">
-        <f>ABS(B31-B32)</f>
         <v>1.6000000000000042E-3</v>
       </c>
       <c r="L31" s="8">
-        <f>A32-A31</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M31" s="1">
-        <f>ABS(C32-C31)</f>
+        <f t="shared" si="3"/>
         <v>1.9999999999999948E-3</v>
       </c>
-      <c r="O31" s="16" t="s">
+      <c r="O31" s="14" t="s">
         <v>13</v>
       </c>
       <c r="P31" t="s">
@@ -5530,7 +5674,7 @@
         <v>B*10^-5</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>600</v>
       </c>
@@ -5541,45 +5685,45 @@
         <v>4.7300000000000002E-2</v>
       </c>
       <c r="D32">
+        <f t="shared" si="4"/>
+        <v>5.7666666666666668E-5</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="5"/>
+        <v>7.883333333333333E-5</v>
+      </c>
+      <c r="I32" s="8">
         <f t="shared" si="0"/>
-        <v>5.7666666666666668E-5</v>
-      </c>
-      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="J32">
         <f t="shared" si="1"/>
-        <v>7.883333333333333E-5</v>
-      </c>
-      <c r="I32" s="8">
-        <f>A33-A32</f>
-        <v>20</v>
-      </c>
-      <c r="J32">
-        <f>ABS(B32-B33)</f>
         <v>1.0999999999999968E-3</v>
       </c>
       <c r="L32" s="8">
-        <f>A33-A32</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M32" s="1">
-        <f>ABS(C33-C32)</f>
+        <f t="shared" si="3"/>
         <v>1.800000000000003E-3</v>
       </c>
-      <c r="O32" s="15">
-        <v>6.9375499999999998E-3</v>
+      <c r="O32">
+        <v>8.0490000000000006E-3</v>
       </c>
       <c r="P32">
         <f>O32^2</f>
-        <v>4.8129600002499995E-5</v>
+        <v>6.478640100000001E-5</v>
       </c>
       <c r="Q32">
         <v>11</v>
       </c>
       <c r="R32">
         <f>P32*10^5</f>
-        <v>4.8129600002499995</v>
+        <v>6.4786401000000007</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>620</v>
       </c>
@@ -5590,11 +5734,11 @@
         <v>4.5499999999999999E-2</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5.4032258064516134E-5</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7.3387096774193552E-5</v>
       </c>
       <c r="I33" s="8"/>
@@ -5606,19 +5750,19 @@
         <f>MAX(M2:M32)</f>
         <v>8.0100000000000005E-2</v>
       </c>
-      <c r="O33" s="15">
-        <v>7.8868989999999993E-3</v>
+      <c r="O33">
+        <v>8.2939999999999993E-3</v>
       </c>
       <c r="P33">
         <f>O33^2</f>
-        <v>6.2203175836200988E-5</v>
+        <v>6.879043599999999E-5</v>
       </c>
       <c r="Q33">
         <v>13</v>
       </c>
       <c r="R33">
         <f>P33*10^5</f>
-        <v>6.2203175836200986</v>
+        <v>6.8790435999999993</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -5636,12 +5780,19 @@
       </c>
       <c r="P35">
         <f>P33-P32</f>
-        <v>1.4073575833700993E-5</v>
+        <v>4.0040349999999797E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <f>O35/P35</f>
+        <v>499496.1332755608</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>